<commit_message>
make some datasets for R and Python
</commit_message>
<xml_diff>
--- a/input/codebooks/設問対応表（作成途中）.xlsx
+++ b/input/codebooks/設問対応表（作成途中）.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chika/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chika/data_todai-asahi/input/codebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{516CFD1E-3F0D-B049-8DA4-590486DF83AE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{82AAAD4D-2DD3-9144-A2E2-CCD9F1E7E8FB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15020" yWindow="460" windowWidth="13300" windowHeight="14420" xr2:uid="{12E73871-0DFD-9542-8BA2-562C95AD2E3E}"/>
+    <workbookView xWindow="14020" yWindow="460" windowWidth="13300" windowHeight="14420" xr2:uid="{12E73871-0DFD-9542-8BA2-562C95AD2E3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -595,7 +595,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="802">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="803">
   <si>
     <t>id</t>
   </si>
@@ -4345,6 +4345,13 @@
     <t>毎月</t>
     <rPh sb="0" eb="2">
       <t>マイツキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>★年によって定義が違うので要確認</t>
+    <rPh sb="0" eb="1">
+      <t>トシ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -4410,7 +4417,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4441,6 +4448,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -4456,7 +4469,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4519,6 +4532,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4836,19 +4855,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55635E95-F044-CE4A-A5C8-B261928C4854}">
   <dimension ref="A1:R219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A186" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C208" sqref="C208"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <cols>
     <col min="3" max="3" width="34" customWidth="1"/>
-    <col min="4" max="5" width="0" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="42.28515625" hidden="1" customWidth="1"/>
-    <col min="7" max="8" width="0" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="55.28515625" hidden="1" customWidth="1"/>
-    <col min="10" max="11" width="0" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="50.5703125" style="5" hidden="1" customWidth="1"/>
+    <col min="4" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" customWidth="1"/>
+    <col min="7" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="55.28515625" customWidth="1"/>
+    <col min="10" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="50.5703125" style="5" customWidth="1"/>
     <col min="15" max="15" width="55.42578125" customWidth="1"/>
     <col min="18" max="18" width="47.7109375" customWidth="1"/>
   </cols>
@@ -5324,39 +5343,42 @@
         <v>439</v>
       </c>
     </row>
-    <row r="17" spans="4:18">
-      <c r="D17" t="s">
+    <row r="17" spans="3:18" s="21" customFormat="1">
+      <c r="C17" s="21" t="s">
+        <v>802</v>
+      </c>
+      <c r="D17" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="21" t="s">
         <v>366</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="21" t="s">
         <v>366</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="L17" s="22" t="s">
         <v>440</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="O17" t="s">
+      <c r="O17" s="21" t="s">
         <v>440</v>
       </c>
-      <c r="P17" t="s">
+      <c r="P17" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="R17" t="s">
+      <c r="R17" s="21" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="19" spans="4:18">
+    <row r="19" spans="3:18">
       <c r="D19" s="14" t="s">
         <v>411</v>
       </c>
@@ -5374,7 +5396,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="20" spans="4:18">
+    <row r="20" spans="3:18">
       <c r="D20" t="s">
         <v>34</v>
       </c>
@@ -5403,7 +5425,7 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="4:18">
+    <row r="21" spans="3:18">
       <c r="D21" s="14" t="s">
         <v>368</v>
       </c>
@@ -5440,7 +5462,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="22" spans="4:18">
+    <row r="22" spans="3:18">
       <c r="D22" t="s">
         <v>35</v>
       </c>
@@ -5481,7 +5503,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="23" spans="4:18">
+    <row r="23" spans="3:18">
       <c r="D23" t="s">
         <v>36</v>
       </c>
@@ -5519,7 +5541,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="24" spans="4:18">
+    <row r="24" spans="3:18">
       <c r="D24" s="14" t="s">
         <v>371</v>
       </c>
@@ -5541,7 +5563,7 @@
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="4:18">
+    <row r="25" spans="3:18">
       <c r="D25" t="s">
         <v>37</v>
       </c>
@@ -5573,7 +5595,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="26" spans="4:18">
+    <row r="26" spans="3:18">
       <c r="D26" t="s">
         <v>38</v>
       </c>
@@ -5605,7 +5627,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="27" spans="4:18">
+    <row r="27" spans="3:18">
       <c r="D27" s="14" t="s">
         <v>374</v>
       </c>
@@ -5633,7 +5655,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="28" spans="4:18">
+    <row r="28" spans="3:18">
       <c r="D28" t="s">
         <v>39</v>
       </c>
@@ -5661,7 +5683,7 @@
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="4:18">
+    <row r="29" spans="3:18">
       <c r="D29" t="s">
         <v>40</v>
       </c>
@@ -5702,7 +5724,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="30" spans="4:18">
+    <row r="30" spans="3:18">
       <c r="D30" t="s">
         <v>41</v>
       </c>
@@ -5743,7 +5765,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="31" spans="4:18">
+    <row r="31" spans="3:18">
       <c r="G31" t="s">
         <v>69</v>
       </c>
@@ -5778,7 +5800,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="32" spans="4:18">
+    <row r="32" spans="3:18">
       <c r="G32" s="14" t="s">
         <v>418</v>
       </c>

</xml_diff>